<commit_message>
Metadeconfound R for report
</commit_message>
<xml_diff>
--- a/metadata_hiperammon.xlsx
+++ b/metadata_hiperammon.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitatdevalencia-my.sharepoint.com/personal/logipe_alumni_uv_es/Documents/Doctorado/Estudios/CIPF_2022/Analisis_resultados_ratas_hiperammon/Rats_HE_HiperAmmon_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_3A039F163278F7B706DCC6EF9D31867776B61F6F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C83CED6-7D0F-CD43-A827-8B7D40C4B22E}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_3A039F163278F7B706DCC6EF9D31867776B61F6F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CA3E921-987E-FF40-AA5E-594F5DEA683D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -204,10 +207,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -245,7 +252,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -351,7 +358,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,7 +500,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -504,7 +511,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B23" sqref="B23:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -732,27 +739,27 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1">
-        <v>104</v>
+        <v>95.4</v>
       </c>
       <c r="E14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -761,29 +768,29 @@
         <v>116</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="1">
-        <v>98.4</v>
+        <v>104</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -792,7 +799,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="1">
-        <v>61.6</v>
+        <v>104</v>
       </c>
       <c r="E17" t="s">
         <v>22</v>
@@ -800,7 +807,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -809,7 +816,7 @@
         <v>7</v>
       </c>
       <c r="D18" s="1">
-        <v>98.6</v>
+        <v>116</v>
       </c>
       <c r="E18" t="s">
         <v>22</v>
@@ -817,7 +824,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -826,7 +833,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="1">
-        <v>120</v>
+        <v>98.4</v>
       </c>
       <c r="E19" t="s">
         <v>22</v>
@@ -834,16 +841,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="1">
-        <v>110</v>
+        <v>61.6</v>
       </c>
       <c r="E20" t="s">
         <v>22</v>
@@ -851,16 +858,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="1">
-        <v>116</v>
+        <v>98.6</v>
       </c>
       <c r="E21" t="s">
         <v>22</v>
@@ -868,16 +875,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="1">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="E22" t="s">
         <v>22</v>
@@ -885,7 +892,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
         <v>40</v>
@@ -894,7 +901,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="1">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E23" t="s">
         <v>22</v>
@@ -902,7 +909,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
@@ -911,7 +918,7 @@
         <v>7</v>
       </c>
       <c r="D24" s="1">
-        <v>85.8</v>
+        <v>116</v>
       </c>
       <c r="E24" t="s">
         <v>22</v>
@@ -919,7 +926,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
@@ -928,7 +935,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="1">
-        <v>72.2</v>
+        <v>104</v>
       </c>
       <c r="E25" t="s">
         <v>22</v>
@@ -936,7 +943,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
@@ -945,15 +952,15 @@
         <v>7</v>
       </c>
       <c r="D26" s="1">
-        <v>95.4</v>
+        <v>100</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
@@ -962,15 +969,15 @@
         <v>7</v>
       </c>
       <c r="D27" s="1">
-        <v>116</v>
+        <v>85.8</v>
       </c>
       <c r="E27" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -979,10 +986,10 @@
         <v>7</v>
       </c>
       <c r="D28" s="1">
-        <v>104</v>
+        <v>72.2</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -1003,6 +1010,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E29">
+      <sortCondition ref="E1:E29"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>